<commit_message>
merge coords in a single column using a geopoint
A recent addition to Table Schema.
</commit_message>
<xml_diff>
--- a/exemple-valide.xlsx
+++ b/exemple-valide.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -31,10 +31,7 @@
     <t xml:space="preserve">insee</t>
   </si>
   <si>
-    <t xml:space="preserve">xlong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ylat</t>
+    <t xml:space="preserve">geopoint</t>
   </si>
   <si>
     <t xml:space="preserve">adresse</t>
@@ -55,10 +52,7 @@
     <t xml:space="preserve">Vallier</t>
   </si>
   <si>
-    <t xml:space="preserve">5.7118754</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.1800016</t>
+    <t xml:space="preserve">5.7118754, 45.1800016</t>
   </si>
   <si>
     <t xml:space="preserve">Boulevard Joseph Vallier</t>
@@ -70,28 +64,19 @@
     <t xml:space="preserve">Gare – Frise</t>
   </si>
   <si>
-    <t xml:space="preserve">5.71363</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.19129</t>
+    <t xml:space="preserve">5.71363, 45.19129</t>
   </si>
   <si>
     <t xml:space="preserve">Rue de la Frise</t>
   </si>
   <si>
-    <t xml:space="preserve">0476544254</t>
-  </si>
-  <si>
     <t xml:space="preserve">38185-T-003</t>
   </si>
   <si>
     <t xml:space="preserve">Gare – Emile Gueymard</t>
   </si>
   <si>
-    <t xml:space="preserve">5.715028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.191447</t>
+    <t xml:space="preserve">5.715028, 45.191447</t>
   </si>
   <si>
     <t xml:space="preserve">Rue Emile Gueymard</t>
@@ -103,10 +88,7 @@
     <t xml:space="preserve">Gare – Casimir Brenier</t>
   </si>
   <si>
-    <t xml:space="preserve">5.715636</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.191326</t>
+    <t xml:space="preserve">5.715636, 45.191326</t>
   </si>
   <si>
     <t xml:space="preserve">Rue Casimir Brenier</t>
@@ -118,10 +100,7 @@
     <t xml:space="preserve">Lorraine</t>
   </si>
   <si>
-    <t xml:space="preserve">5.715604</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.189905</t>
+    <t xml:space="preserve">5.715604, 45.189905</t>
   </si>
   <si>
     <t xml:space="preserve">Place de la Gare</t>
@@ -133,10 +112,7 @@
     <t xml:space="preserve">Victor Hugo</t>
   </si>
   <si>
-    <t xml:space="preserve">5.724516</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.189495</t>
+    <t xml:space="preserve">5.724516, 45.189495</t>
   </si>
   <si>
     <t xml:space="preserve">Place Victor Hugo</t>
@@ -148,10 +124,7 @@
     <t xml:space="preserve">Joffre</t>
   </si>
   <si>
-    <t xml:space="preserve">5.7325</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.18401</t>
+    <t xml:space="preserve">5.7325, 45.18401</t>
   </si>
   <si>
     <t xml:space="preserve">Boulevard Marechal Joffre</t>
@@ -163,10 +136,7 @@
     <t xml:space="preserve">Ambroise Croizat</t>
   </si>
   <si>
-    <t xml:space="preserve">5.7529</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.1842</t>
+    <t xml:space="preserve">5.7529, 45.1842</t>
   </si>
   <si>
     <t xml:space="preserve">Avenue Ambroise Croizat</t>
@@ -178,10 +148,7 @@
     <t xml:space="preserve">Grand Place</t>
   </si>
   <si>
-    <t xml:space="preserve">5.73187</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.15934</t>
+    <t xml:space="preserve">5.73187, 45.15934</t>
   </si>
   <si>
     <t xml:space="preserve">Avenue de l’Europe</t>
@@ -193,10 +160,7 @@
     <t xml:space="preserve">Esmonin</t>
   </si>
   <si>
-    <t xml:space="preserve">5.728535</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.15876</t>
+    <t xml:space="preserve">5.728535, 45.15876</t>
   </si>
   <si>
     <t xml:space="preserve">Avenue Edmond Esmonin</t>
@@ -208,10 +172,7 @@
     <t xml:space="preserve">Gresivaudan-Aiguinards</t>
   </si>
   <si>
-    <t xml:space="preserve">5.762533</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.210125</t>
+    <t xml:space="preserve">5.762533, 45.210125</t>
   </si>
   <si>
     <t xml:space="preserve">Avenue du Gresivaudan</t>
@@ -223,10 +184,7 @@
     <t xml:space="preserve">Gare de Moirans</t>
   </si>
   <si>
-    <t xml:space="preserve">5.5819</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.3224</t>
+    <t xml:space="preserve">5.5819, 45.3224</t>
   </si>
   <si>
     <t xml:space="preserve">Route de la Gare</t>
@@ -238,10 +196,7 @@
     <t xml:space="preserve">Saint Jean</t>
   </si>
   <si>
-    <t xml:space="preserve">5.632017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.243095</t>
+    <t xml:space="preserve">5.632017, 45.243095</t>
   </si>
   <si>
     <t xml:space="preserve">Avenue Saint Jean</t>
@@ -253,10 +208,7 @@
     <t xml:space="preserve">Vercors</t>
   </si>
   <si>
-    <t xml:space="preserve">5.643157</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.071641</t>
+    <t xml:space="preserve">5.643157, 45.071641</t>
   </si>
   <si>
     <t xml:space="preserve">Route du Vercors</t>
@@ -268,10 +220,7 @@
     <t xml:space="preserve">Uriage</t>
   </si>
   <si>
-    <t xml:space="preserve">5.810867</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.118761</t>
+    <t xml:space="preserve">5.810867, 45.118761</t>
   </si>
   <si>
     <t xml:space="preserve">Avenue d’Uriage</t>
@@ -283,10 +232,7 @@
     <t xml:space="preserve">Joliot-Curie</t>
   </si>
   <si>
-    <t xml:space="preserve">5.870029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.273657</t>
+    <t xml:space="preserve">5.870029, 45.273657</t>
   </si>
   <si>
     <t xml:space="preserve">Avenue Joliot Curie</t>
@@ -298,10 +244,7 @@
     <t xml:space="preserve">Gare de Pontcharra</t>
   </si>
   <si>
-    <t xml:space="preserve">6.008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.434</t>
+    <t xml:space="preserve">6.008, 45.434</t>
   </si>
 </sst>
 </file>
@@ -397,10 +340,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -408,12 +351,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -441,359 +383,305 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="n">
+        <v>38185</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>38185</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="0" t="n">
+      <c r="F2" s="0" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>38185</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>38185</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>19</v>
+      <c r="G3" s="0" t="n">
+        <v>476544254</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>38185</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>38185</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>38185</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>38185</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>38185</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>38421</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>38185</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>38151</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38229</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>38239</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>38281</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38436</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>38529</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="F16" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38039</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>38314</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="F18" s="0" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>